<commit_message>
Changes in WebSite, Color Status logic updated
</commit_message>
<xml_diff>
--- a/Documents/Technical/Design/CompFormStatus.xlsx
+++ b/Documents/Technical/Design/CompFormStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="343"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,28 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
-  <si>
-    <t>Match Not Found</t>
-  </si>
-  <si>
-    <t>Match Found</t>
-  </si>
-  <si>
-    <t>Full</t>
-  </si>
-  <si>
-    <t>Partial</t>
-  </si>
-  <si>
-    <t>Issue Not Identified</t>
-  </si>
-  <si>
-    <t>Isue Identified</t>
-  </si>
-  <si>
-    <t>Review not completed</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="67">
   <si>
     <t>lt green</t>
   </si>
@@ -45,48 +24,215 @@
     <t>lt red</t>
   </si>
   <si>
-    <t>Review Completed</t>
-  </si>
-  <si>
     <t>Issues Identified</t>
   </si>
   <si>
-    <t>Issues not identified</t>
-  </si>
-  <si>
     <t>red</t>
   </si>
   <si>
     <t>green</t>
   </si>
   <si>
-    <t>manual site</t>
-  </si>
-  <si>
     <t>grey</t>
   </si>
   <si>
-    <t>not manual site</t>
-  </si>
-  <si>
-    <t>matches found</t>
-  </si>
-  <si>
-    <t>matches not found</t>
-  </si>
-  <si>
-    <t>Site Search Status</t>
-  </si>
-  <si>
     <t>Investigator</t>
+  </si>
+  <si>
+    <t>Reivew Completed</t>
+  </si>
+  <si>
+    <t>Review Not Completed</t>
+  </si>
+  <si>
+    <t>Issues Not Identified</t>
+  </si>
+  <si>
+    <t>Matches Found</t>
+  </si>
+  <si>
+    <t>Matches not found</t>
+  </si>
+  <si>
+    <t>Comp Form</t>
+  </si>
+  <si>
+    <t>No issues identified</t>
+  </si>
+  <si>
+    <t>one or more issues identifed</t>
+  </si>
+  <si>
+    <t>one or more matches found</t>
+  </si>
+  <si>
+    <t>no match found</t>
+  </si>
+  <si>
+    <t>Search Status</t>
+  </si>
+  <si>
+    <t>Status Enum</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Status Description</t>
+  </si>
+  <si>
+    <t>Extraction Mode - Manual</t>
+  </si>
+  <si>
+    <t>Extraction Mode - Automatic (Scanned)</t>
+  </si>
+  <si>
+    <t>Review Pending, Issues Not Identified (Manual Search)</t>
+  </si>
+  <si>
+    <t>Has Extraction Erros</t>
+  </si>
+  <si>
+    <t>No Extraction Errors</t>
+  </si>
+  <si>
+    <t>Extraction Not Successful</t>
+  </si>
+  <si>
+    <t>Not Extracted</t>
+  </si>
+  <si>
+    <t>No Match Found</t>
+  </si>
+  <si>
+    <t>Partial Match Found</t>
+  </si>
+  <si>
+    <t>Full Match Found</t>
+  </si>
+  <si>
+    <t>Review Pending, Partial Match Found</t>
+  </si>
+  <si>
+    <t>Review Pending, Full Match Found</t>
+  </si>
+  <si>
+    <t>Review Pending, No Match Found</t>
+  </si>
+  <si>
+    <t>Review completed, n Issues Identified</t>
+  </si>
+  <si>
+    <t>Review Completed, Issues not Identified</t>
+  </si>
+  <si>
+    <t>Review Pending, n Issues Identified</t>
+  </si>
+  <si>
+    <t>Issues identified, manual or through matched record, all other checks are ignored after the issues are identified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ReviewCompletedIssuesNotIdentified</t>
+  </si>
+  <si>
+    <t>IssuesIdentifiedReviewPending</t>
+  </si>
+  <si>
+    <t>ManualSearchSiteReviewPending</t>
+  </si>
+  <si>
+    <t>NotScanned</t>
+  </si>
+  <si>
+    <t>HasExtractionErrors</t>
+  </si>
+  <si>
+    <t>NoMatchFoundReviewPending</t>
+  </si>
+  <si>
+    <t>PartialMatchFoundReviewPending</t>
+  </si>
+  <si>
+    <t>FullMatchFoundReviewPending</t>
+  </si>
+  <si>
+    <t>Statement starts with Review Completed because it is a closure statement, thefore Review Completed has higher significance over Issues Identified or Not Identified.</t>
+  </si>
+  <si>
+    <t>ReviewCompletedIssuesIdentified</t>
+  </si>
+  <si>
+    <t>Data Not Extracted</t>
+  </si>
+  <si>
+    <t>Review completed, Issue{1} at {0} Source{1} identified</t>
+  </si>
+  <si>
+    <t>Issue{1} Identified at {0} Source{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>Extraction Error Site Count &gt; 0</t>
+  </si>
+  <si>
+    <t>Extraction Pending Site Count &gt; 0</t>
+  </si>
+  <si>
+    <t>Extraction Error Site Count = 0</t>
+  </si>
+  <si>
+    <t>Data Extraction Error at {0} Source{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>Data Extraction Pending at {0} Source{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>NotScanned;</t>
+  </si>
+  <si>
+    <t>Com Form</t>
+  </si>
+  <si>
+    <t>Review completed, Issue{1} identified for {0} Investigator{1}</t>
+  </si>
+  <si>
+    <t>Issues Identified Investigator Count</t>
+  </si>
+  <si>
+    <t>Issue{1} Identified for {0} Investigator{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>Extraction Pending Investigator Count &gt; 0</t>
+  </si>
+  <si>
+    <t>Data Extraction Error for {0} Investigator{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>Data Not Extracted for {0} Investigator{1}, Review Pending</t>
+  </si>
+  <si>
+    <t>Investigator count = 0</t>
+  </si>
+  <si>
+    <t>Investigator not added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,8 +260,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,133 +565,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E16"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" t="s">
         <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
copied all files form p926-ddas
</commit_message>
<xml_diff>
--- a/Documents/Technical/Design/CompFormStatus.xlsx
+++ b/Documents/Technical/Design/CompFormStatus.xlsx
@@ -567,9 +567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,49 +895,49 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>54</v>
+      <c r="C30" t="s">
+        <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G31" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>29</v>
+      <c r="D32" t="s">
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>